<commit_message>
change mort fig type
</commit_message>
<xml_diff>
--- a/analyses/mort_fig.xlsx
+++ b/analyses/mort_fig.xlsx
@@ -8,13 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6752E7A0-249A-9C4B-A202-81FCBCECC0F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B770CC51-3567-8644-AF54-037D4685FC41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$D$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$4</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$5</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>warm</t>
   </si>
@@ -42,9 +58,6 @@
   </si>
   <si>
     <t>ambient</t>
-  </si>
-  <si>
-    <t>pre-treatment</t>
   </si>
 </sst>
 </file>
@@ -180,8 +193,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -192,23 +206,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pre-treatment</c:v>
+                  <c:v>cold</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
@@ -258,7 +270,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -284,10 +296,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9EF5-5444-B2F2-6D0CE045FFB8}"/>
+              <c16:uniqueId val="{00000000-C749-D242-8D92-004600878459}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -300,23 +311,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cold</c:v>
+                  <c:v>ambient</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
@@ -366,7 +375,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -384,7 +393,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -392,10 +401,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9EF5-5444-B2F2-6D0CE045FFB8}"/>
+              <c16:uniqueId val="{00000001-C749-D242-8D92-004600878459}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -408,23 +416,23 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ambient</c:v>
+                  <c:v>warm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
@@ -477,146 +485,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9EF5-5444-B2F2-6D0CE045FFB8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>warm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$M$2</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>43047</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43048</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43049</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43050</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43051</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43052</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43053</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43054</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43055</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43056</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$6:$M$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9EF5-5444-B2F2-6D0CE045FFB8}"/>
+              <c16:uniqueId val="{00000002-C749-D242-8D92-004600878459}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -624,12 +523,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="768743184"/>
-        <c:axId val="768841584"/>
-      </c:lineChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="735708688"/>
+        <c:axId val="801711792"/>
+      </c:barChart>
       <c:dateAx>
-        <c:axId val="768743184"/>
+        <c:axId val="735708688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,14 +572,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="768841584"/>
+        <c:crossAx val="801711792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="768841584"/>
+        <c:axId val="801711792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="768743184"/>
+        <c:crossAx val="735708688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -858,7 +758,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -966,11 +866,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -981,11 +876,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1017,9 +907,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1377,23 +1264,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A08FFEF-8778-A54A-BAA9-947AD811D6CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0F24BB7-9F8A-5E48-B07A-CD12EF4C254E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1714,7 +1601,7 @@
   <dimension ref="A2:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1760,10 +1647,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="C3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1789,10 +1676,10 @@
     </row>
     <row r="4" spans="1:16">
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
         <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1810,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1818,59 +1705,30 @@
     </row>
     <row r="5" spans="1:16">
       <c r="C5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>27</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-      <c r="L6">
-        <v>7</v>
-      </c>
-      <c r="M6">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save changes to excel file
</commit_message>
<xml_diff>
--- a/analyses/mort_fig.xlsx
+++ b/analyses/mort_fig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B770CC51-3567-8644-AF54-037D4685FC41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26921D00-0987-F240-9671-35847E3FF790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
+    <workbookView xWindow="25600" yWindow="1640" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1601,7 +1601,7 @@
   <dimension ref="A2:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
save changes to make new survival figure
</commit_message>
<xml_diff>
--- a/analyses/mort_fig.xlsx
+++ b/analyses/mort_fig.xlsx
@@ -8,29 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26921D00-0987-F240-9671-35847E3FF790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461647D7-00A8-754E-9CF1-A10948959ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="1640" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$D$2:$M$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$3:$M$3</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$4:$M$4</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$5:$M$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$M$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$3:$M$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$4:$M$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$5:$M$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$5</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -100,10 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,64 +120,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number of mortalities</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8208184396982673E-2"/>
+          <c:y val="0.116386542591267"/>
+          <c:w val="0.78870619363209649"/>
+          <c:h val="0.7161581961345741"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -228,37 +168,37 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$M$2</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43047</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43048</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43049</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43050</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43051</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43052</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43053</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43054</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43055</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43056</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,37 +273,37 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$M$2</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43047</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43048</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43049</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43050</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43051</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43052</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43053</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43054</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43055</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43056</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,37 +380,37 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$M$2</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43047</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43048</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43049</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43050</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43051</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43052</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43053</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43054</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43055</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43056</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,14 +468,69 @@
         <c:axId val="735708688"/>
         <c:axId val="801711792"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="735708688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -575,9 +570,10 @@
         <c:crossAx val="801711792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="801711792"/>
         <c:scaling>
@@ -599,6 +595,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Number of mortalities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.3618103875949266E-3"/>
+              <c:y val="0.282995943688857"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -644,6 +703,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86950237238115835"/>
+          <c:y val="0.27121665473633977"/>
+          <c:w val="0.13013903552847494"/>
+          <c:h val="0.31363183011214513"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -657,7 +726,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1598,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4373F3-0706-6F4B-8761-8123A90CA41E}">
-  <dimension ref="A2:P14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1609,37 +1678,66 @@
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:16">
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1">
+        <v>4</v>
+      </c>
+      <c r="I1">
+        <v>5</v>
+      </c>
+      <c r="J1">
+        <v>6</v>
+      </c>
+      <c r="K1">
+        <v>7</v>
+      </c>
+      <c r="L1">
+        <v>8</v>
+      </c>
+      <c r="M1">
+        <v>9</v>
+      </c>
+    </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1"/>
       <c r="D2" s="2">
-        <v>43047</v>
-      </c>
-      <c r="E2" s="1">
-        <v>43048</v>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>43049</v>
-      </c>
-      <c r="G2" s="1">
-        <v>43050</v>
-      </c>
-      <c r="H2" s="1">
-        <v>43051</v>
-      </c>
-      <c r="I2" s="1">
-        <v>43052</v>
-      </c>
-      <c r="J2" s="1">
-        <v>43053</v>
-      </c>
-      <c r="K2" s="1">
-        <v>43054</v>
-      </c>
-      <c r="L2" s="1">
-        <v>43055</v>
-      </c>
-      <c r="M2" s="1">
-        <v>43056</v>
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>6</v>
+      </c>
+      <c r="K2" s="3">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3">
+        <v>9</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>

</xml_diff>

<commit_message>
save changes to mortality figure
</commit_message>
<xml_diff>
--- a/analyses/mort_fig.xlsx
+++ b/analyses/mort_fig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461647D7-00A8-754E-9CF1-A10948959ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C4E882-987E-0442-BFFA-CBF48323CC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="1640" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>warm</t>
+    <t>4 ˚C</t>
   </si>
   <si>
-    <t>cold</t>
+    <t>7.5 ˚C</t>
   </si>
   <si>
-    <t>ambient</t>
+    <t>10 ˚C</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cold</c:v>
+                  <c:v>4 ˚C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -251,7 +251,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ambient</c:v>
+                  <c:v>7.5 ˚C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -356,7 +356,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>warm</c:v>
+                  <c:v>10 ˚C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1669,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4373F3-0706-6F4B-8761-8123A90CA41E}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="C5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>0</v>

</xml_diff>

<commit_message>
edit survival figure - font size and axis
</commit_message>
<xml_diff>
--- a/analyses/mort_fig.xlsx
+++ b/analyses/mort_fig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C4E882-987E-0442-BFFA-CBF48323CC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC960295-2650-6342-A7DF-9008D63BED28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="25040" windowHeight="14300" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
   </bookViews>
@@ -84,11 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,10 +167,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$M$2</c:f>
+              <c:f>Sheet1!$D$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -199,16 +200,40 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$M$3</c:f>
+              <c:f>Sheet1!$D$3:$U$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
@@ -231,6 +256,30 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -271,10 +320,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$M$2</c:f>
+              <c:f>Sheet1!$D$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -304,16 +353,40 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$M$4</c:f>
+              <c:f>Sheet1!$D$4:$U$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
@@ -336,6 +409,30 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -378,10 +475,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$M$2</c:f>
+              <c:f>Sheet1!$D$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -411,16 +508,40 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$M$5</c:f>
+              <c:f>Sheet1!$D$5:$U$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
@@ -444,6 +565,30 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,7 +627,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -495,12 +640,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Day</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46974418927971084"/>
+              <c:y val="0.91823196543329033"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -514,7 +667,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -552,7 +705,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -602,7 +755,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -615,7 +768,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Number of mortalities</a:t>
                 </a:r>
               </a:p>
@@ -625,8 +778,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="9.3618103875949266E-3"/>
-              <c:y val="0.282995943688857"/>
+              <c:x val="2.9413177285423598E-3"/>
+              <c:y val="0.28299585462680682"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -642,7 +795,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -674,7 +827,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -726,7 +879,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1340,9 +1493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1667,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4373F3-0706-6F4B-8761-8123A90CA41E}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1678,7 +1831,7 @@
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:21">
       <c r="E1">
         <v>1</v>
       </c>
@@ -1707,7 +1860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:21">
       <c r="A2" s="1"/>
       <c r="D2" s="2">
         <v>0</v>
@@ -1739,11 +1892,32 @@
       <c r="M2" s="3">
         <v>9</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="N2" s="4">
+        <v>10</v>
+      </c>
+      <c r="O2" s="4">
+        <v>11</v>
+      </c>
+      <c r="P2" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>13</v>
+      </c>
+      <c r="R2" s="4">
+        <v>14</v>
+      </c>
+      <c r="S2" s="4">
+        <v>15</v>
+      </c>
+      <c r="T2" s="4">
+        <v>16</v>
+      </c>
+      <c r="U2" s="4">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:21">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -1771,8 +1945,32 @@
       <c r="M3">
         <v>0</v>
       </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:21">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -1800,8 +1998,32 @@
       <c r="M4">
         <v>0</v>
       </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:21">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -1829,23 +2051,47 @@
       <c r="M5">
         <v>3</v>
       </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:21">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:21">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:21">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:21">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:21">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:21">
       <c r="A14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save kap meier survival fig  to images and xcel sheet used to create it
</commit_message>
<xml_diff>
--- a/analyses/mort_fig.xlsx
+++ b/analyses/mort_fig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23BDF39-ADEC-1C4B-8BC5-5494CF12275E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71EBF94-3B5B-3D4E-A669-1249344DF687}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="25540" windowHeight="14740" activeTab="2" xr2:uid="{15B09E9E-3F1B-6E49-A220-729973E3E891}"/>
   </bookViews>
@@ -5001,7 +5001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F21CC33-D5C4-B34A-B9EE-567F14A58D4C}">
   <dimension ref="B1:X63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <selection activeCell="E29" sqref="E29:E63"/>
     </sheetView>
   </sheetViews>
@@ -6945,7 +6945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10C0A5F-3762-C148-9360-EF8EDA4F6CF2}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q8" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>

</xml_diff>